<commit_message>
Zeitplan und Arbeitsjournal aktualisiert
</commit_message>
<xml_diff>
--- a/planen/Zeitplan.xlsx
+++ b/planen/Zeitplan.xlsx
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:AR79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2925,8 +2925,8 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -3015,7 +3015,7 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
+      <c r="N37" s="11"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
@@ -3103,7 +3103,7 @@
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
+      <c r="N39" s="11"/>
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
@@ -3191,8 +3191,8 @@
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
@@ -4897,22 +4897,25 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
@@ -4925,25 +4928,22 @@
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:O1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="74" orientation="landscape" horizontalDpi="300" r:id="rId1"/>

</xml_diff>